<commit_message>
tna report has been updated
</commit_message>
<xml_diff>
--- a/public/template/tna-report.xlsx
+++ b/public/template/tna-report.xlsx
@@ -1,44 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\form files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7450" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Start date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end date </t>
+    <t>Name En</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
   <si>
     <t>Venue</t>
+  </si>
+  <si>
+    <t>softbd</t>
+  </si>
+  <si>
+    <t>dhaka</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -61,14 +89,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF6A8759"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -91,39 +193,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -202,194 +304,194 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="3" max="4" width="12.6328125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="13">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6">
+        <v>37511</v>
+      </c>
+      <c r="D2" s="6">
+        <v>40149</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>